<commit_message>
add project to list
</commit_message>
<xml_diff>
--- a/docs/ListofProjects.xlsx
+++ b/docs/ListofProjects.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\course52311\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9315"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Student ID</t>
   </si>
@@ -54,17 +49,29 @@
   </si>
   <si>
     <t>Michael Bell</t>
+  </si>
+  <si>
+    <t>Bendel Dan</t>
+  </si>
+  <si>
+    <t>Testing independence using random projections</t>
+  </si>
+  <si>
+    <t>matlab</t>
+  </si>
+  <si>
+    <t>Fainblat Ido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -73,7 +80,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -373,7 +380,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -381,23 +388,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>36507473</v>
       </c>
@@ -432,6 +439,34 @@
       </c>
       <c r="E2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>21924816</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>38000014</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>